<commit_message>
start tests from console
</commit_message>
<xml_diff>
--- a/epg_tests.xlsx
+++ b/epg_tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Каналы" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Раздел</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t xml:space="preserve">DDT: 45, </t>
+  </si>
+  <si>
+    <t>46 настройка параметры запуска в командной строке</t>
+  </si>
+  <si>
+    <t>не запускаются тесты в chrome из консоли</t>
   </si>
 </sst>
 </file>
@@ -429,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,18 +489,18 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K3" t="s">
-        <v>18</v>
+      <c r="K3" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -508,7 +514,17 @@
         <v>15</v>
       </c>
       <c r="K5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
data package, channels module
</commit_message>
<xml_diff>
--- a/epg_tests.xlsx
+++ b/epg_tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Раздел</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>чтобы тесты запускались из консоли, необоходимо в PATH положить драйвера chromedriver.exe, IEDriverServer.exe</t>
+  </si>
+  <si>
+    <t>Магия pytest_generate_tests: 57 с 3:20</t>
+  </si>
+  <si>
+    <t>Магия с фикстурой pytest: 18 с 08:28</t>
   </si>
 </sst>
 </file>
@@ -439,7 +445,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,10 +503,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K4" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -515,17 +518,17 @@
         <v>15</v>
       </c>
       <c r="K5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -539,6 +542,16 @@
         <v>15</v>
       </c>
       <c r="K8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
channels load from json
</commit_message>
<xml_diff>
--- a/epg_tests.xlsx
+++ b/epg_tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Раздел</t>
   </si>
@@ -81,9 +81,6 @@
     <t xml:space="preserve">DDT: 45, </t>
   </si>
   <si>
-    <t>46 настройка параметры запуска в командной строке</t>
-  </si>
-  <si>
     <t>сделать fixture.channel.count() из DB</t>
   </si>
   <si>
@@ -94,6 +91,18 @@
   </si>
   <si>
     <t>Магия с фикстурой pytest: 18 с 08:28</t>
+  </si>
+  <si>
+    <t>параметры запуска в командной строке: 46</t>
+  </si>
+  <si>
+    <t>json: 50, 56, 58</t>
+  </si>
+  <si>
+    <t>конвертер xls to json</t>
+  </si>
+  <si>
+    <t>в env проекта должны быть: putest, webdriver, jsonpickle</t>
   </si>
 </sst>
 </file>
@@ -442,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +513,12 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -517,9 +531,6 @@
       <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="K5" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K6" t="s">
@@ -528,7 +539,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K7" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -542,22 +553,37 @@
         <v>15</v>
       </c>
       <c r="K8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K13" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create channel + db assert = ok
</commit_message>
<xml_diff>
--- a/epg_tests.xlsx
+++ b/epg_tests.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -69,9 +69,6 @@
     <t>Разное</t>
   </si>
   <si>
-    <t>избавиться от sleep()</t>
-  </si>
-  <si>
     <t>лекции про строки: 39-44</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>прикрутить unicode (падает при наличии каналов с кириллицей в имени)</t>
+  </si>
+  <si>
+    <t>избавиться от sleep(). При отсутствии sleep(1) после создания канала, слишком рано берется из БД новый список каналов</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,17 +514,17 @@
         <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
         <v>15</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -554,52 +554,52 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nose create and del channel tests working!
</commit_message>
<xml_diff>
--- a/epg_tests.xlsx
+++ b/epg_tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Раздел</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Фикстуры, маркировка тестов: Юнит тестирование в Python (10_07-09)</t>
+  </si>
+  <si>
+    <t>nose-parameterized - для параметризованных тестов</t>
   </si>
 </sst>
 </file>
@@ -466,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,6 +627,11 @@
     <row r="22" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K22" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
half a way to success with banners
</commit_message>
<xml_diff>
--- a/epg_tests.xlsx
+++ b/epg_tests.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="разное" sheetId="2" r:id="rId1"/>
     <sheet name="Каналы" sheetId="1" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="решения" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>Раздел</t>
   </si>
@@ -118,6 +118,87 @@
   </si>
   <si>
     <t>в env проекта должны быть: pytest/nosetest, webdriver, jsonpickle, psycopg2, requests, nose-parameterized</t>
+  </si>
+  <si>
+    <t>Необходимо загрузить файл на сервер, используя стандартные элементы HTML:</t>
+  </si>
+  <si>
+    <t>&lt;input name="uploadFile" type="file"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;input name="doUpload" value="Upload" type="button"/&gt;</t>
+  </si>
+  <si>
+    <t>Решение:</t>
+  </si>
+  <si>
+    <t>Я рекомендую просто взять и вынести себе это в отдельный универсальный метод и использовать его каждый раз когда нужно что-либо загрузить через такую форму.</t>
+  </si>
+  <si>
+    <t>Исключение:</t>
+  </si>
+  <si>
+    <t>Safari Driver полностью не поддерживает загрузку файла, т.к. насколько я понял, он javascript-based. Появляющееся окно с выбором файла ставит его в тупиковое положение. Такие сценарии нужно либо избегать, либо добиваться результата другим способом — создавать собственный HTTP запрос или подкладывать данные напрямую на стороне сервера, если такая возможность имеется.</t>
+  </si>
+  <si>
+    <t>Пример кода:</t>
+  </si>
+  <si>
+    <t>protected void uploadFile(By uploadInput, By uploadButton, String filePath) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        clearInput(uploadInput);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        findElement(uploadInput).sendKeys(filePath);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        findElement(uploadButton).click();</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>Действия с элементами внутри iframe</t>
+  </si>
+  <si>
+    <t>Проблема:</t>
+  </si>
+  <si>
+    <t>Если требуемый элемент находится внутри iframe — он не доступен из дефолтного контекста. Вы не сможете обнаружить его в DOM модели и webDriver будет бросать исключение NoSuchElementException.</t>
+  </si>
+  <si>
+    <t>Перед тем как взаимодействовать с этим элементом, необходимо переключить webDriver на контекст iframe элемента. Как я понимаю, это связано с тем, что контекст страницы и контекст iframe на этой странице — это две разных DOM модели.</t>
+  </si>
+  <si>
+    <t>webDriver.switchTo().frame(findElement(By.id("id_of_your_iframe")));</t>
+  </si>
+  <si>
+    <t>// do actions against inner web element, located in iframe</t>
+  </si>
+  <si>
+    <t>webDriver.switchTo().defaultContent();</t>
+  </si>
+  <si>
+    <t>// continue to do actions in default content</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>http://barancev.github.io/slow-loading-pages/</t>
+  </si>
+  <si>
+    <t>DRAG&amp;DROP, 11-04 Поляруш: from selenium.webdriver import ActionChains</t>
+  </si>
+  <si>
+    <t>+ Поляруш 11-04 38:00</t>
+  </si>
+  <si>
+    <t>driver.execute_script(js_script)</t>
+  </si>
+  <si>
+    <t>driver.execute_script("window.scrollTo(0, 1000);")</t>
   </si>
 </sst>
 </file>
@@ -168,10 +249,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -475,7 +557,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -661,12 +745,160 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
progress in channels model and fill form (OK)
</commit_message>
<xml_diff>
--- a/epg_tests.xlsx
+++ b/epg_tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="разное" sheetId="2" r:id="rId1"/>
@@ -117,9 +117,6 @@
     <t>WebDriverWait - вместо sleep()</t>
   </si>
   <si>
-    <t>в env проекта должны быть: pytest/nosetest, webdriver, jsonpickle, psycopg2, requests, nose-parameterized</t>
-  </si>
-  <si>
     <t>Необходимо загрузить файл на сервер, используя стандартные элементы HTML:</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>driver.execute_script("window.scrollTo(0, 1000);")</t>
+  </si>
+  <si>
+    <t>в env проекта должны быть: pytest/nosetest, selenium, jsonpickle, psycopg2, requests, nose-parameterized, pyautogui (+image)</t>
   </si>
 </sst>
 </file>
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +645,7 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -747,7 +747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
@@ -755,147 +755,147 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
provider, banners validation - OK
</commit_message>
<xml_diff>
--- a/epg_tests.xlsx
+++ b/epg_tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="разное" sheetId="2" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>Реализовать</t>
   </si>
   <si>
-    <t>fixture.channel.count()</t>
-  </si>
-  <si>
     <t>Разное</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>в env проекта должны быть: pytest/nosetest, selenium, jsonpickle, psycopg2, requests, nose-parameterized, pyautogui (+image)</t>
+  </si>
+  <si>
+    <t>добавление каналов через апи</t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -565,92 +565,92 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -734,7 +734,7 @@
         <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -755,147 +755,147 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add channels via rest - OK
</commit_message>
<xml_diff>
--- a/epg_tests.xlsx
+++ b/epg_tests.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830"/>
   </bookViews>
   <sheets>
-    <sheet name="разное" sheetId="2" r:id="rId1"/>
-    <sheet name="Каналы" sheetId="1" r:id="rId2"/>
+    <sheet name="Каналы" sheetId="1" r:id="rId1"/>
+    <sheet name="разное" sheetId="2" r:id="rId2"/>
     <sheet name="решения" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>Раздел</t>
   </si>
@@ -198,14 +198,23 @@
     <t>в env проекта должны быть: pytest/nosetest, selenium, jsonpickle, psycopg2, requests, nose-parameterized, pyautogui (+image)</t>
   </si>
   <si>
-    <t>добавление каналов через апи</t>
+    <t>тесты со спецсимволами</t>
+  </si>
+  <si>
+    <t>app.create_random_channel() - сделать через REST</t>
+  </si>
+  <si>
+    <t>кириллица</t>
+  </si>
+  <si>
+    <t>парсер параметров командной строки</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +230,13 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="3">
@@ -249,11 +265,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -555,116 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A22"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,8 +635,18 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -734,7 +657,113 @@
         <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
negative tests for channel
</commit_message>
<xml_diff>
--- a/epg_tests.xlsx
+++ b/epg_tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>Раздел</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>генератор jpeg (pil?)</t>
+  </si>
+  <si>
+    <t>xls - json adapter</t>
   </si>
 </sst>
 </file>
@@ -574,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,6 +664,11 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addd negative tests - OK
</commit_message>
<xml_diff>
--- a/epg_tests.xlsx
+++ b/epg_tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>Раздел</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>xls - json adapter</t>
+  </si>
+  <si>
+    <t>DDT вместо parametrized? https://pypi.python.org/pypi/ddt</t>
   </si>
 </sst>
 </file>
@@ -577,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,6 +672,11 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>